<commit_message>
added groc fixed october 2022 snafu
</commit_message>
<xml_diff>
--- a/A2/data/uberdash.xlsx
+++ b/A2/data/uberdash.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="4">
   <si>
     <t>YYMM</t>
   </si>
@@ -24,6 +24,9 @@
   </si>
   <si>
     <t>SPEND_AMOUNT</t>
+  </si>
+  <si>
+    <t>Unnamed: 3</t>
   </si>
 </sst>
 </file>
@@ -428,7 +431,7 @@
         <v>2167780.8</v>
       </c>
       <c r="C4">
-        <v>68244709.13000001</v>
+        <v>68244709.11999999</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -439,7 +442,7 @@
         <v>2056277.85</v>
       </c>
       <c r="C5">
-        <v>64339464.13999999</v>
+        <v>64339464.20000002</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -450,7 +453,7 @@
         <v>2302475.210000001</v>
       </c>
       <c r="C6">
-        <v>72433065.34000003</v>
+        <v>72433065.29000002</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -472,7 +475,7 @@
         <v>2367173.619999999</v>
       </c>
       <c r="C8">
-        <v>73103432.73999995</v>
+        <v>73103432.77999997</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -483,7 +486,7 @@
         <v>2542516.209999999</v>
       </c>
       <c r="C9">
-        <v>77135047.42000002</v>
+        <v>77135047.39999998</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -494,7 +497,7 @@
         <v>2628500.73</v>
       </c>
       <c r="C10">
-        <v>79303082.92999995</v>
+        <v>79303082.89999998</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -505,7 +508,7 @@
         <v>2817597.710000001</v>
       </c>
       <c r="C11">
-        <v>85827325.34000003</v>
+        <v>85827325.39999998</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -516,7 +519,7 @@
         <v>2698233.910000004</v>
       </c>
       <c r="C12">
-        <v>84346802.27999997</v>
+        <v>84346802.20000005</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -527,7 +530,7 @@
         <v>2735202.519999996</v>
       </c>
       <c r="C13">
-        <v>87457261.26999998</v>
+        <v>87457261.29999995</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -549,7 +552,7 @@
         <v>3020246.44</v>
       </c>
       <c r="C15">
-        <v>95192460.30999999</v>
+        <v>95192460.33999999</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -560,7 +563,7 @@
         <v>3380604.99</v>
       </c>
       <c r="C16">
-        <v>111952800.23</v>
+        <v>111952800.2</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -615,7 +618,7 @@
         <v>7042967.989999998</v>
       </c>
       <c r="C21">
-        <v>237625455.1999998</v>
+        <v>237625455.6099999</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -626,7 +629,7 @@
         <v>7041927.870000005</v>
       </c>
       <c r="C22">
-        <v>229289794.4100001</v>
+        <v>229289794</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -637,7 +640,7 @@
         <v>7794592.039999992</v>
       </c>
       <c r="C23">
-        <v>255090913.21</v>
+        <v>255090913</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -648,7 +651,7 @@
         <v>7539076.330000013</v>
       </c>
       <c r="C24">
-        <v>248271130.25</v>
+        <v>248271130</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -659,7 +662,7 @@
         <v>8210834.549999997</v>
       </c>
       <c r="C25">
-        <v>276198420.8000002</v>
+        <v>276198421</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -670,7 +673,7 @@
         <v>9324708.59</v>
       </c>
       <c r="C26">
-        <v>314656599.77</v>
+        <v>314656599.8</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -681,7 +684,7 @@
         <v>8316655.019999996</v>
       </c>
       <c r="C27">
-        <v>278654048.64</v>
+        <v>278654048.6</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -692,7 +695,7 @@
         <v>9592401.400000006</v>
       </c>
       <c r="C28">
-        <v>319326490.15</v>
+        <v>319326490.2</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -703,7 +706,7 @@
         <v>9659053.370000001</v>
       </c>
       <c r="C29">
-        <v>323398158.54</v>
+        <v>323398158.4</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -714,7 +717,7 @@
         <v>9879211.789999999</v>
       </c>
       <c r="C30">
-        <v>333916388.6500001</v>
+        <v>333916389</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -725,7 +728,7 @@
         <v>9256773.869999997</v>
       </c>
       <c r="C31">
-        <v>306876533.9400003</v>
+        <v>306876533.6900003</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -736,7 +739,7 @@
         <v>9689090.959999993</v>
       </c>
       <c r="C32">
-        <v>321985059.0199997</v>
+        <v>321985059.3099997</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -747,7 +750,7 @@
         <v>9731515.160000004</v>
       </c>
       <c r="C33">
-        <v>322088494.4500003</v>
+        <v>322088494.1600003</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -758,7 +761,7 @@
         <v>9476757.920000002</v>
       </c>
       <c r="C34">
-        <v>313324738.3599997</v>
+        <v>313324738.8399997</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -769,7 +772,7 @@
         <v>10106286.93000001</v>
       </c>
       <c r="C35">
-        <v>336797364.1399999</v>
+        <v>336797364</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -777,10 +780,10 @@
         <v>2111</v>
       </c>
       <c r="B36">
-        <v>9626952.479999989</v>
+        <v>9626952.489999995</v>
       </c>
       <c r="C36">
-        <v>321331607.1300001</v>
+        <v>321331607</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -788,10 +791,10 @@
         <v>2112</v>
       </c>
       <c r="B37">
-        <v>10134213.63000001</v>
+        <v>10134213.59999999</v>
       </c>
       <c r="C37">
-        <v>343800779.4000001</v>
+        <v>343800779</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -802,7 +805,7 @@
         <v>10737733.56</v>
       </c>
       <c r="C38">
-        <v>365342652.27</v>
+        <v>365342652.3</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -813,7 +816,7 @@
         <v>9803648.179999998</v>
       </c>
       <c r="C39">
-        <v>330918924.9299999</v>
+        <v>330918924.8999999</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -824,7 +827,7 @@
         <v>11007359.95</v>
       </c>
       <c r="C40">
-        <v>370481533.2500001</v>
+        <v>370481532.8000001</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -835,7 +838,7 @@
         <v>10870999.71</v>
       </c>
       <c r="C41">
-        <v>370048781.6099999</v>
+        <v>370048782</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -846,7 +849,7 @@
         <v>11120525.64999999</v>
       </c>
       <c r="C42">
-        <v>381151540.5599999</v>
+        <v>381151540.6199999</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -857,7 +860,7 @@
         <v>10356081.22000001</v>
       </c>
       <c r="C43">
-        <v>353226014.54</v>
+        <v>353226014.3800001</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -868,7 +871,7 @@
         <v>10534225.85</v>
       </c>
       <c r="C44">
-        <v>364289811.73</v>
+        <v>364289812</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -879,7 +882,7 @@
         <v>10340266.98999999</v>
       </c>
       <c r="C45">
-        <v>356142623.9100003</v>
+        <v>356142624</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -887,10 +890,10 @@
         <v>2209</v>
       </c>
       <c r="B46">
-        <v>0</v>
+        <v>10308955.07000001</v>
       </c>
       <c r="C46">
-        <v>0</v>
+        <v>353876016</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -898,10 +901,10 @@
         <v>2210</v>
       </c>
       <c r="B47">
-        <v>10308955.07000001</v>
+        <v>10869381.41999999</v>
       </c>
       <c r="C47">
-        <v>353876016.3299999</v>
+        <v>374789342</v>
       </c>
     </row>
     <row r="48" spans="1:3">
@@ -909,10 +912,10 @@
         <v>2211</v>
       </c>
       <c r="B48">
-        <v>21295055.53999999</v>
+        <v>10425674.10000001</v>
       </c>
       <c r="C48">
-        <v>733688579.5999999</v>
+        <v>358899237.73</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -920,7 +923,7 @@
         <v>2212</v>
       </c>
       <c r="B49">
-        <v>10898187.11</v>
+        <v>10898187.13</v>
       </c>
       <c r="C49">
         <v>381187263.2200007</v>
@@ -934,7 +937,7 @@
         <v>11132507.81</v>
       </c>
       <c r="C50">
-        <v>385847187.36</v>
+        <v>385847187.4</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -945,7 +948,7 @@
         <v>10725060.22</v>
       </c>
       <c r="C51">
-        <v>370191995.72</v>
+        <v>370191995.7</v>
       </c>
     </row>
     <row r="52" spans="1:3">
@@ -956,7 +959,7 @@
         <v>12118193.57</v>
       </c>
       <c r="C52">
-        <v>416408720.9299999</v>
+        <v>416408720.9</v>
       </c>
     </row>
     <row r="53" spans="1:3">
@@ -967,7 +970,7 @@
         <v>11704519.33</v>
       </c>
       <c r="C53">
-        <v>404036293.4199998</v>
+        <v>404036293.4299998</v>
       </c>
     </row>
     <row r="54" spans="1:3">
@@ -978,7 +981,7 @@
         <v>11909004.61000001</v>
       </c>
       <c r="C54">
-        <v>411526873.7200003</v>
+        <v>411526873.5700002</v>
       </c>
     </row>
     <row r="55" spans="1:3">
@@ -989,7 +992,7 @@
         <v>11541955.32000001</v>
       </c>
       <c r="C55">
-        <v>396539587.2599998</v>
+        <v>396539587</v>
       </c>
     </row>
     <row r="56" spans="1:3">
@@ -1000,7 +1003,7 @@
         <v>11733139.49999999</v>
       </c>
       <c r="C56">
-        <v>407758990.25</v>
+        <v>407758991</v>
       </c>
     </row>
     <row r="57" spans="1:3">
@@ -1011,7 +1014,7 @@
         <v>11495455.41</v>
       </c>
       <c r="C57">
-        <v>395753325.5300002</v>
+        <v>395753325</v>
       </c>
     </row>
     <row r="58" spans="1:3">
@@ -1022,7 +1025,7 @@
         <v>11530493.17</v>
       </c>
       <c r="C58">
-        <v>395633410.0800004</v>
+        <v>395633410.2700005</v>
       </c>
     </row>
     <row r="59" spans="1:3">
@@ -1041,7 +1044,7 @@
         <v>2311</v>
       </c>
       <c r="B60">
-        <v>11295149.84999999</v>
+        <v>11295149.90000001</v>
       </c>
       <c r="C60">
         <v>390802479.7600007</v>
@@ -1052,7 +1055,7 @@
         <v>2312</v>
       </c>
       <c r="B61">
-        <v>12068675.15000001</v>
+        <v>12068675.09999999</v>
       </c>
       <c r="C61">
         <v>424318668.1899986</v>
@@ -1077,7 +1080,7 @@
         <v>11961648.9</v>
       </c>
       <c r="C63">
-        <v>417453068.7599999</v>
+        <v>417453068.72</v>
       </c>
     </row>
     <row r="64" spans="1:3">
@@ -1088,7 +1091,7 @@
         <v>13249620.92</v>
       </c>
       <c r="C64">
-        <v>462026821.34</v>
+        <v>462026821.4</v>
       </c>
     </row>
     <row r="65" spans="1:3">
@@ -1099,7 +1102,7 @@
         <v>12715074.32</v>
       </c>
       <c r="C65">
-        <v>439918083.8200002</v>
+        <v>439918083.8000002</v>
       </c>
     </row>
     <row r="66" spans="1:3">
@@ -1132,7 +1135,7 @@
         <v>12700391.09999998</v>
       </c>
       <c r="C68">
-        <v>442249556.2999992</v>
+        <v>442249556.3899994</v>
       </c>
     </row>
     <row r="69" spans="1:3">
@@ -1143,7 +1146,7 @@
         <v>12845531.24000001</v>
       </c>
       <c r="C69">
-        <v>447279830.2200003</v>
+        <v>447279830</v>
       </c>
     </row>
     <row r="70" spans="1:3">
@@ -1151,10 +1154,10 @@
         <v>2409</v>
       </c>
       <c r="B70">
-        <v>12398684.13</v>
+        <v>12398684.09999999</v>
       </c>
       <c r="C70">
-        <v>432660425.04</v>
+        <v>432660425</v>
       </c>
     </row>
     <row r="71" spans="1:3">
@@ -1162,10 +1165,10 @@
         <v>2410</v>
       </c>
       <c r="B71">
-        <v>12914607.54000001</v>
+        <v>12914607.60000001</v>
       </c>
       <c r="C71">
-        <v>450245499.9300003</v>
+        <v>450245500</v>
       </c>
     </row>
     <row r="72" spans="1:3">
@@ -1173,10 +1176,10 @@
         <v>2411</v>
       </c>
       <c r="B72">
-        <v>12747305.03</v>
+        <v>12747305</v>
       </c>
       <c r="C72">
-        <v>449028644.8199997</v>
+        <v>449028645</v>
       </c>
     </row>
     <row r="73" spans="1:3">
@@ -1184,10 +1187,10 @@
         <v>2412</v>
       </c>
       <c r="B73">
-        <v>13184010.78999999</v>
+        <v>13184010.79999998</v>
       </c>
       <c r="C73">
-        <v>473612484.9699993</v>
+        <v>473612484.8899994</v>
       </c>
     </row>
     <row r="74" spans="1:3">
@@ -1198,7 +1201,7 @@
         <v>13312602.35</v>
       </c>
       <c r="C74">
-        <v>473375846.93</v>
+        <v>473375846.9</v>
       </c>
     </row>
     <row r="75" spans="1:3">
@@ -1209,7 +1212,7 @@
         <v>12602778.89</v>
       </c>
       <c r="C75">
-        <v>451204963.2600001</v>
+        <v>451204963.2900001</v>
       </c>
     </row>
     <row r="76" spans="1:3">
@@ -1272,10 +1275,10 @@
         <v>2508</v>
       </c>
       <c r="B81">
-        <v>14325866.43000001</v>
+        <v>14325866.47</v>
       </c>
       <c r="C81">
-        <v>516968612.6900005</v>
+        <v>516968612.2300005</v>
       </c>
     </row>
   </sheetData>
@@ -1285,13 +1288,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C81"/>
+  <dimension ref="A1:D81"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1301,8 +1304,11 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2">
         <v>1901</v>
       </c>
@@ -1313,7 +1319,7 @@
         <v>48804671.12</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:4">
       <c r="A3">
         <v>1902</v>
       </c>
@@ -1324,7 +1330,7 @@
         <v>48501532.14000001</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:4">
       <c r="A4">
         <v>1903</v>
       </c>
@@ -1332,10 +1338,10 @@
         <v>2595405.859999999</v>
       </c>
       <c r="C4">
-        <v>54012045.05999999</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+        <v>54012045.04000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5">
         <v>1904</v>
       </c>
@@ -1343,10 +1349,10 @@
         <v>2678300.540000001</v>
       </c>
       <c r="C5">
-        <v>52282240.44</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+        <v>52282240.45999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6">
         <v>1905</v>
       </c>
@@ -1357,7 +1363,7 @@
         <v>50193495.75</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:4">
       <c r="A7">
         <v>1906</v>
       </c>
@@ -1365,10 +1371,10 @@
         <v>2110965.569999998</v>
       </c>
       <c r="C7">
-        <v>39943646.12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
+        <v>39943646.09000003</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8">
         <v>1907</v>
       </c>
@@ -1376,10 +1382,10 @@
         <v>1686629.109999999</v>
       </c>
       <c r="C8">
-        <v>31431968.25999999</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+        <v>31431968.29999995</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9">
         <v>1908</v>
       </c>
@@ -1387,10 +1393,10 @@
         <v>1944931.070000002</v>
       </c>
       <c r="C9">
-        <v>39897479.00999999</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
+        <v>39897479</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10">
         <v>1909</v>
       </c>
@@ -1398,10 +1404,10 @@
         <v>2359683.040000003</v>
       </c>
       <c r="C10">
-        <v>51902411.13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
+        <v>51902411.10000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11">
         <v>1910</v>
       </c>
@@ -1409,10 +1415,10 @@
         <v>2428830.439999994</v>
       </c>
       <c r="C11">
-        <v>54407014.82000005</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
+        <v>54407014.89999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12">
         <v>1911</v>
       </c>
@@ -1420,10 +1426,10 @@
         <v>2368350.920000002</v>
       </c>
       <c r="C12">
-        <v>54672489.21999997</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
+        <v>54672489.20000005</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13">
         <v>1912</v>
       </c>
@@ -1431,10 +1437,10 @@
         <v>2250574.040000003</v>
       </c>
       <c r="C13">
-        <v>57042329.57000011</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
+        <v>57042329.54000008</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14">
         <v>2001</v>
       </c>
@@ -1445,7 +1451,7 @@
         <v>56103286.78999999</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:4">
       <c r="A15">
         <v>2002</v>
       </c>
@@ -1456,7 +1462,7 @@
         <v>55216865.69999999</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:4">
       <c r="A16">
         <v>2003</v>
       </c>
@@ -1508,7 +1514,7 @@
         <v>4287951.440000001</v>
       </c>
       <c r="C20">
-        <v>122836415.55</v>
+        <v>122836415.51</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -1519,7 +1525,7 @@
         <v>4870404.180000003</v>
       </c>
       <c r="C21">
-        <v>127960387.96</v>
+        <v>127960388</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -1541,7 +1547,7 @@
         <v>4950061.120000005</v>
       </c>
       <c r="C23">
-        <v>136129154.0699999</v>
+        <v>136129154.3599999</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -1552,7 +1558,7 @@
         <v>4807487.509999998</v>
       </c>
       <c r="C24">
-        <v>133846309.8800001</v>
+        <v>133846309.5900002</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -1563,7 +1569,7 @@
         <v>4676539.75</v>
       </c>
       <c r="C25">
-        <v>135404066.0699999</v>
+        <v>135404066.4099998</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -1596,7 +1602,7 @@
         <v>5445607.299999997</v>
       </c>
       <c r="C28">
-        <v>156113589.2699999</v>
+        <v>156113589.2899999</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -1607,7 +1613,7 @@
         <v>5359527.960000001</v>
       </c>
       <c r="C29">
-        <v>152682319.1899999</v>
+        <v>152682319.17</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -1618,7 +1624,7 @@
         <v>5471150.550000001</v>
       </c>
       <c r="C30">
-        <v>159059851.74</v>
+        <v>159059851.73</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -1629,7 +1635,7 @@
         <v>5462179.040000003</v>
       </c>
       <c r="C31">
-        <v>156111480.8200001</v>
+        <v>156111480.83</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -1651,7 +1657,7 @@
         <v>5962079.929999992</v>
       </c>
       <c r="C33">
-        <v>169907582.84</v>
+        <v>169907582.61</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -1662,7 +1668,7 @@
         <v>5792694.960000001</v>
       </c>
       <c r="C34">
-        <v>163862509.6100001</v>
+        <v>163862509.8400002</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -1673,7 +1679,7 @@
         <v>6423717.229999997</v>
       </c>
       <c r="C35">
-        <v>177597265.1899998</v>
+        <v>177597265.1599998</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -1684,7 +1690,7 @@
         <v>6068440.520000003</v>
       </c>
       <c r="C36">
-        <v>166229189.0799999</v>
+        <v>166229189.1099999</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -1706,7 +1712,7 @@
         <v>6459790.720000001</v>
       </c>
       <c r="C38">
-        <v>186130025.41</v>
+        <v>186130025.4</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -1728,7 +1734,7 @@
         <v>6624290.180000003</v>
       </c>
       <c r="C40">
-        <v>188891670.6199999</v>
+        <v>188891670.6</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -1739,7 +1745,7 @@
         <v>6328256.390000001</v>
       </c>
       <c r="C41">
-        <v>184212486.1200001</v>
+        <v>184212486.1500001</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -1761,7 +1767,7 @@
         <v>5942514.039999999</v>
       </c>
       <c r="C43">
-        <v>175875548.5199997</v>
+        <v>175875548.2299998</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -1772,7 +1778,7 @@
         <v>6237315.420000002</v>
       </c>
       <c r="C44">
-        <v>183771367.5799999</v>
+        <v>183771368</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -1783,7 +1789,7 @@
         <v>6162987.280000001</v>
       </c>
       <c r="C45">
-        <v>179451891.3300002</v>
+        <v>179451891</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -1791,10 +1797,10 @@
         <v>2209</v>
       </c>
       <c r="B46">
-        <v>0</v>
+        <v>6019439.979999997</v>
       </c>
       <c r="C46">
-        <v>0</v>
+        <v>176514471</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -1802,10 +1808,10 @@
         <v>2210</v>
       </c>
       <c r="B47">
-        <v>6019439.979999997</v>
+        <v>6331139.729999997</v>
       </c>
       <c r="C47">
-        <v>176514470.6299999</v>
+        <v>185736573</v>
       </c>
     </row>
     <row r="48" spans="1:3">
@@ -1813,10 +1819,10 @@
         <v>2211</v>
       </c>
       <c r="B48">
-        <v>11909705.07999999</v>
+        <v>5578565.350000009</v>
       </c>
       <c r="C48">
-        <v>359800853.45</v>
+        <v>174064280</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -1824,10 +1830,10 @@
         <v>2212</v>
       </c>
       <c r="B49">
-        <v>5411334.800000012</v>
+        <v>5411334.799999997</v>
       </c>
       <c r="C49">
-        <v>182863161.5600002</v>
+        <v>182863162</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -1860,7 +1866,7 @@
         <v>6001661.780000001</v>
       </c>
       <c r="C52">
-        <v>198821285.7399999</v>
+        <v>198821285.7699999</v>
       </c>
     </row>
     <row r="53" spans="1:3">
@@ -1871,7 +1877,7 @@
         <v>5788788.729999999</v>
       </c>
       <c r="C53">
-        <v>193013656.74</v>
+        <v>193013656.7</v>
       </c>
     </row>
     <row r="54" spans="1:3">
@@ -1882,7 +1888,7 @@
         <v>5844180.710000001</v>
       </c>
       <c r="C54">
-        <v>194812830.5600002</v>
+        <v>194812830.5700002</v>
       </c>
     </row>
     <row r="55" spans="1:3">
@@ -1893,7 +1899,7 @@
         <v>5654613.289999999</v>
       </c>
       <c r="C55">
-        <v>189554022.8499999</v>
+        <v>189554022.4299998</v>
       </c>
     </row>
     <row r="56" spans="1:3">
@@ -1904,7 +1910,7 @@
         <v>5758276.579999998</v>
       </c>
       <c r="C56">
-        <v>194728051.4499998</v>
+        <v>194728052</v>
       </c>
     </row>
     <row r="57" spans="1:3">
@@ -1915,7 +1921,7 @@
         <v>5729866.560000002</v>
       </c>
       <c r="C57">
-        <v>190577163.0200002</v>
+        <v>190577162.8900001</v>
       </c>
     </row>
     <row r="58" spans="1:3">
@@ -1926,7 +1932,7 @@
         <v>5848785.640000001</v>
       </c>
       <c r="C58">
-        <v>195160017.8399999</v>
+        <v>195160018.1099999</v>
       </c>
     </row>
     <row r="59" spans="1:3">
@@ -1937,7 +1943,7 @@
         <v>6119673.630000003</v>
       </c>
       <c r="C59">
-        <v>202385409.4200001</v>
+        <v>202385409</v>
       </c>
     </row>
     <row r="60" spans="1:3">
@@ -1948,7 +1954,7 @@
         <v>5601581.239999995</v>
       </c>
       <c r="C60">
-        <v>187986616.3099999</v>
+        <v>187986616</v>
       </c>
     </row>
     <row r="61" spans="1:3">
@@ -1959,7 +1965,7 @@
         <v>5808825.839999996</v>
       </c>
       <c r="C61">
-        <v>199707634.2399998</v>
+        <v>199707635</v>
       </c>
     </row>
     <row r="62" spans="1:3">
@@ -1981,7 +1987,7 @@
         <v>5790224.350000001</v>
       </c>
       <c r="C63">
-        <v>198220762.9</v>
+        <v>198220762.89</v>
       </c>
     </row>
     <row r="64" spans="1:3">
@@ -2003,7 +2009,7 @@
         <v>6322818.73</v>
       </c>
       <c r="C65">
-        <v>209985530.8400002</v>
+        <v>209985530.8500001</v>
       </c>
     </row>
     <row r="66" spans="1:3">
@@ -2025,7 +2031,7 @@
         <v>6368496.160000004</v>
       </c>
       <c r="C67">
-        <v>215331303.8100001</v>
+        <v>215331303.65</v>
       </c>
     </row>
     <row r="68" spans="1:3">
@@ -2036,7 +2042,7 @@
         <v>6462275.319999993</v>
       </c>
       <c r="C68">
-        <v>218760042.7900002</v>
+        <v>218760042.9500003</v>
       </c>
     </row>
     <row r="69" spans="1:3">
@@ -2047,7 +2053,7 @@
         <v>6884326.590000004</v>
       </c>
       <c r="C69">
-        <v>238653540.4699998</v>
+        <v>238653540.0499997</v>
       </c>
     </row>
     <row r="70" spans="1:3">
@@ -2058,7 +2064,7 @@
         <v>6763985.43</v>
       </c>
       <c r="C70">
-        <v>237419822.1799998</v>
+        <v>237419822.5999999</v>
       </c>
     </row>
     <row r="71" spans="1:3">
@@ -2069,7 +2075,7 @@
         <v>6869724.910000004</v>
       </c>
       <c r="C71">
-        <v>240657337.3200002</v>
+        <v>240657337.4000001</v>
       </c>
     </row>
     <row r="72" spans="1:3">
@@ -2080,7 +2086,7 @@
         <v>6681343.689999998</v>
       </c>
       <c r="C72">
-        <v>237233258.3600001</v>
+        <v>237233258</v>
       </c>
     </row>
     <row r="73" spans="1:3">
@@ -2091,7 +2097,7 @@
         <v>6833607.730000004</v>
       </c>
       <c r="C73">
-        <v>247731498.4000001</v>
+        <v>247731498.6800003</v>
       </c>
     </row>
     <row r="74" spans="1:3">
@@ -2124,7 +2130,7 @@
         <v>7417159.739999998</v>
       </c>
       <c r="C76">
-        <v>266909264.11</v>
+        <v>266909264.1299999</v>
       </c>
     </row>
     <row r="77" spans="1:3">
@@ -2135,7 +2141,7 @@
         <v>7077686.109999999</v>
       </c>
       <c r="C77">
-        <v>252389623.13</v>
+        <v>252389623.11</v>
       </c>
     </row>
     <row r="78" spans="1:3">
@@ -2146,7 +2152,7 @@
         <v>7407671.350000001</v>
       </c>
       <c r="C78">
-        <v>270334392.59</v>
+        <v>270334393.09</v>
       </c>
     </row>
     <row r="79" spans="1:3">
@@ -2157,7 +2163,7 @@
         <v>6989623.130000003</v>
       </c>
       <c r="C79">
-        <v>257429312.3099999</v>
+        <v>257429312</v>
       </c>
     </row>
     <row r="80" spans="1:3">
@@ -2168,7 +2174,7 @@
         <v>7109510.969999999</v>
       </c>
       <c r="C80">
-        <v>258224971.6500006</v>
+        <v>258224971.4600005</v>
       </c>
     </row>
     <row r="81" spans="1:3">
@@ -2179,7 +2185,7 @@
         <v>7346493.859999999</v>
       </c>
       <c r="C81">
-        <v>267283138.5799994</v>
+        <v>267283138.5399995</v>
       </c>
     </row>
   </sheetData>

</xml_diff>